<commit_message>
100% translated / starting revision
</commit_message>
<xml_diff>
--- a/tradept/Excel/Localization/Main/english/S商人列表_MerchantItems_hotfix.xlsx
+++ b/tradept/Excel/Localization/Main/english/S商人列表_MerchantItems_hotfix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\tradesp\Excel\Localization\Main\english\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\tradept\Excel\Localization\Main\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D550D0A-29C3-4EFB-ABC3-0EF7E5F5D7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968B4779-FC74-4CB5-AE12-2282CB2A4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -208,16 +208,16 @@
     <t>魔晶商人</t>
   </si>
   <si>
-    <t>Comerciante</t>
-  </si>
-  <si>
-    <t>Boticario itinerante</t>
-  </si>
-  <si>
-    <t>Comerciante de Montura</t>
-  </si>
-  <si>
-    <t>Comerciante de Joyas</t>
+    <t>Homem de negocios</t>
+  </si>
+  <si>
+    <t>boticário itinerante</t>
+  </si>
+  <si>
+    <t>Comerciante de Montaria</t>
+  </si>
+  <si>
+    <t>Comerciante de joias</t>
   </si>
 </sst>
 </file>
@@ -352,39 +352,39 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="普通" xfId="2" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="普通 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
@@ -735,11 +735,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="23.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75">
       <c r="A1" s="7" t="s">

</xml_diff>